<commit_message>
Fixed graph, edited formatting
</commit_message>
<xml_diff>
--- a/Graphs for Report.xlsx
+++ b/Graphs for Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Krithik\Documents\GitHub\ee209-2020-project-team02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A7A4B1F-D303-43E1-B3D6-33B63732B2A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B388DB-F23B-4D7E-957D-EBE4DCEFD891}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D31E458-EF34-49A4-9E1D-C32283C7CB9A}"/>
   </bookViews>
@@ -136,12 +136,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -167,12 +174,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -195,40 +209,62 @@
             <c:v>ADC Voltage</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
             </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
               </a:effectLst>
             </c:spPr>
           </c:marker>
@@ -239,10 +275,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>-6.06</c:v>
+                  <c:v>8.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.100000000000001</c:v>
+                  <c:v>13.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>18.399999999999999</c:v>
@@ -266,7 +302,7 @@
                   <c:v>5.34</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2.72</c:v>
+                  <c:v>-1.49</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>-8.07</c:v>
@@ -281,7 +317,7 @@
                   <c:v>-21.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-21.7</c:v>
+                  <c:v>-21.6</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>-20.100000000000001</c:v>
@@ -327,10 +363,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -345,7 +380,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -376,7 +411,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1">
                       <a:lumMod val="75000"/>
@@ -396,8 +431,12 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -435,10 +474,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -453,7 +491,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -484,7 +522,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1">
                       <a:lumMod val="75000"/>
@@ -511,7 +549,6 @@
                 <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -547,7 +584,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -588,20 +625,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -644,12 +689,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -675,12 +727,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -703,40 +762,62 @@
             <c:v>ADC Current</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent2">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
             </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
               </a:effectLst>
             </c:spPr>
           </c:marker>
@@ -831,6 +912,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -838,7 +933,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -853,7 +948,6 @@
                   <a:rPr lang="en-NZ"/>
                   <a:t>Data Points</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-NZ" baseline="0"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -870,7 +964,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1">
                       <a:lumMod val="75000"/>
@@ -890,8 +984,12 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -929,10 +1027,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -947,7 +1044,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -960,13 +1057,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-NZ"/>
-                  <a:t>Current,</a:t>
+                  <a:t>Current, A</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-NZ" baseline="0"/>
-                  <a:t> A</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-NZ"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -983,7 +1075,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1">
                       <a:lumMod val="75000"/>
@@ -1010,7 +1102,6 @@
                 <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1046,7 +1137,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1087,20 +1178,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -3643,1082 +3742,6 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="15000"/>
-        <a:lumOff val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="139700">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="14000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:lumMod val="60000"/>
-          <a:lumOff val="40000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="15000"/>
-        <a:lumOff val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="139700">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="14000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:lumMod val="60000"/>
-          <a:lumOff val="40000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5220,7 +4243,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5722,7 +4745,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6224,20 +5247,1024 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>252412</xdr:colOff>
+      <xdr:colOff>252413</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>358020</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>24848</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6264,16 +6291,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>252412</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>180881</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>17450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>454321</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6712,8 +6739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5D2BA0-9362-4A35-A13E-FD63B2012518}">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6739,7 +6766,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-6.06</v>
+        <v>8.15</v>
       </c>
       <c r="B2">
         <v>0.06</v>
@@ -6747,7 +6774,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>16.100000000000001</v>
+        <v>13.9</v>
       </c>
       <c r="B3">
         <v>0.16</v>
@@ -6811,7 +6838,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>-2.72</v>
+        <v>-1.49</v>
       </c>
       <c r="B11">
         <v>0.02</v>
@@ -6851,7 +6878,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>-21.7</v>
+        <v>-21.6</v>
       </c>
       <c r="B16">
         <v>-0.28000000000000003</v>

</xml_diff>

<commit_message>
Added graphs to show peak accuracy without peak detector, added slide for project management
</commit_message>
<xml_diff>
--- a/Graphs for Report.xlsx
+++ b/Graphs for Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\ee209-2020-project-team02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Krithik\Documents\GitHub\ee209-2020-project-team02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EA6FE8-C435-4ECA-A7E3-5BCD3525FD0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9641767C-0FE7-4824-A580-81273AF9298B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{6D31E458-EF34-49A4-9E1D-C32283C7CB9A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D31E458-EF34-49A4-9E1D-C32283C7CB9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>ADC Voltage</a:t>
+              <a:t>ADC Voltage @ 50Hz</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -747,7 +747,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>ADC Current</a:t>
+              <a:t>ADC Current @ 50Hz</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -13409,24 +13409,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5D2BA0-9362-4A35-A13E-FD63B2012518}">
   <dimension ref="A1:AI147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R45" sqref="R45"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83984375" customWidth="1"/>
-    <col min="2" max="2" width="18.83984375" customWidth="1"/>
-    <col min="4" max="4" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.15625" customWidth="1"/>
-    <col min="7" max="7" width="14.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="15" max="15" width="18.68359375" customWidth="1"/>
-    <col min="16" max="16" width="21.15625" customWidth="1"/>
-    <col min="17" max="17" width="19.26171875" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -13434,7 +13434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8.15</v>
       </c>
@@ -13442,7 +13442,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13.9</v>
       </c>
@@ -13450,7 +13450,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>18.399999999999999</v>
       </c>
@@ -13458,7 +13458,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>21.1</v>
       </c>
@@ -13466,7 +13466,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>21.7</v>
       </c>
@@ -13474,7 +13474,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20.100000000000001</v>
       </c>
@@ -13482,7 +13482,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>16.600000000000001</v>
       </c>
@@ -13490,7 +13490,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11.5</v>
       </c>
@@ -13498,7 +13498,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5.34</v>
       </c>
@@ -13506,7 +13506,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-1.49</v>
       </c>
@@ -13514,7 +13514,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-8.07</v>
       </c>
@@ -13522,7 +13522,7 @@
         <v>-0.06</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-13.9</v>
       </c>
@@ -13530,7 +13530,7 @@
         <v>-0.14000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-18.399999999999999</v>
       </c>
@@ -13538,7 +13538,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-21.1</v>
       </c>
@@ -13546,7 +13546,7 @@
         <v>-0.26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-21.6</v>
       </c>
@@ -13554,7 +13554,7 @@
         <v>-0.28000000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-20.100000000000001</v>
       </c>
@@ -13562,7 +13562,7 @@
         <v>-0.27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-16.600000000000001</v>
       </c>
@@ -13570,7 +13570,7 @@
         <v>-0.24</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-11.5</v>
       </c>
@@ -13578,7 +13578,7 @@
         <v>-0.18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-5.27</v>
       </c>
@@ -13586,7 +13586,7 @@
         <v>-0.11</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>15.4</v>
       </c>
@@ -13597,7 +13597,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -13641,7 +13641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>15.8</v>
       </c>
@@ -13701,7 +13701,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>15.3</v>
       </c>
@@ -13762,7 +13762,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>15.3</v>
       </c>
@@ -13823,7 +13823,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15.3</v>
       </c>
@@ -13883,7 +13883,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>15.3</v>
       </c>
@@ -13943,7 +13943,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>15.3</v>
       </c>
@@ -14003,7 +14003,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>15.3</v>
       </c>
@@ -14063,7 +14063,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>15.3</v>
       </c>
@@ -14124,7 +14124,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>15.3</v>
       </c>
@@ -14184,7 +14184,7 @@
         <v>-0.64</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>15.3</v>
       </c>
@@ -14244,7 +14244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>15.3</v>
       </c>
@@ -14304,7 +14304,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>15.3</v>
       </c>
@@ -14364,7 +14364,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>15.3</v>
       </c>
@@ -14424,7 +14424,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>15.3</v>
       </c>
@@ -14484,7 +14484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>15.3</v>
       </c>
@@ -14544,7 +14544,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>14.9</v>
       </c>
@@ -14604,7 +14604,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>15.3</v>
       </c>
@@ -14664,7 +14664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>15.3</v>
       </c>
@@ -14724,7 +14724,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>15.3</v>
       </c>
@@ -14784,7 +14784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>15.3</v>
       </c>
@@ -14844,7 +14844,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>15.3</v>
       </c>
@@ -14904,7 +14904,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>15.3</v>
       </c>
@@ -14964,7 +14964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>15.2</v>
       </c>
@@ -15024,7 +15024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>15.3</v>
       </c>
@@ -15084,7 +15084,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>15.3</v>
       </c>
@@ -15144,7 +15144,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>15.3</v>
       </c>
@@ -15204,7 +15204,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>15.3</v>
       </c>
@@ -15264,7 +15264,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>15.3</v>
       </c>
@@ -15324,7 +15324,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>15.3</v>
       </c>
@@ -15384,7 +15384,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>15.3</v>
       </c>
@@ -15444,7 +15444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>15.3</v>
       </c>
@@ -15504,7 +15504,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>15.3</v>
       </c>
@@ -15564,7 +15564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>15.3</v>
       </c>
@@ -15624,7 +15624,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>15.3</v>
       </c>
@@ -15684,7 +15684,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>15.3</v>
       </c>
@@ -15744,7 +15744,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>15.3</v>
       </c>
@@ -15804,7 +15804,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>15.3</v>
       </c>
@@ -15864,7 +15864,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>15.3</v>
       </c>
@@ -15924,7 +15924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>15.3</v>
       </c>
@@ -15984,7 +15984,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>15.3</v>
       </c>
@@ -16044,7 +16044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>15.3</v>
       </c>
@@ -16104,7 +16104,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>15.3</v>
       </c>
@@ -16164,7 +16164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>15.3</v>
       </c>
@@ -16224,7 +16224,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>15.3</v>
       </c>
@@ -16284,7 +16284,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>15.2</v>
       </c>
@@ -16344,7 +16344,7 @@
         <v>-0.24</v>
       </c>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>15.3</v>
       </c>
@@ -16404,7 +16404,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>15.3</v>
       </c>
@@ -16464,7 +16464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>15.3</v>
       </c>
@@ -16524,7 +16524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>15.3</v>
       </c>
@@ -16584,7 +16584,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
       <c r="M97" s="1">
         <v>14.5</v>
       </c>
@@ -16607,7 +16607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>3</v>
       </c>
@@ -16636,7 +16636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>12.6</v>
       </c>
@@ -16662,7 +16662,7 @@
         <v>-0.24</v>
       </c>
     </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>12.6</v>
       </c>
@@ -16688,7 +16688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>12.6</v>
       </c>
@@ -16714,7 +16714,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>12.6</v>
       </c>
@@ -16740,7 +16740,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="103" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>12.6</v>
       </c>
@@ -16766,7 +16766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>12.6</v>
       </c>
@@ -16792,7 +16792,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="105" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>12.6</v>
       </c>
@@ -16818,7 +16818,7 @@
         <v>-0.19</v>
       </c>
     </row>
-    <row r="106" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>12.6</v>
       </c>
@@ -16844,7 +16844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>12.6</v>
       </c>
@@ -16870,7 +16870,7 @@
         <v>-0.19</v>
       </c>
     </row>
-    <row r="108" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>12.6</v>
       </c>
@@ -16896,7 +16896,7 @@
         <v>-0.17</v>
       </c>
     </row>
-    <row r="109" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>12.6</v>
       </c>
@@ -16922,7 +16922,7 @@
         <v>-0.17</v>
       </c>
     </row>
-    <row r="110" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>12.6</v>
       </c>
@@ -16948,7 +16948,7 @@
         <v>-0.34</v>
       </c>
     </row>
-    <row r="111" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>12.6</v>
       </c>
@@ -16974,7 +16974,7 @@
         <v>-0.33</v>
       </c>
     </row>
-    <row r="112" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>12.6</v>
       </c>
@@ -17000,7 +17000,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="113" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>12.6</v>
       </c>
@@ -17026,7 +17026,7 @@
         <v>-0.64</v>
       </c>
     </row>
-    <row r="114" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>12.6</v>
       </c>
@@ -17038,7 +17038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>12.6</v>
       </c>
@@ -17050,7 +17050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B116">
         <v>12.6</v>
       </c>
@@ -17062,7 +17062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B117">
         <v>12.6</v>
       </c>
@@ -17074,7 +17074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B118">
         <v>12.6</v>
       </c>
@@ -17086,7 +17086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B119">
         <v>12.6</v>
       </c>
@@ -17098,7 +17098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B120">
         <v>12.6</v>
       </c>
@@ -17110,7 +17110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>12.6</v>
       </c>
@@ -17122,7 +17122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>12.6</v>
       </c>
@@ -17134,7 +17134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>12.6</v>
       </c>
@@ -17146,7 +17146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>12.6</v>
       </c>
@@ -17158,7 +17158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>12.6</v>
       </c>
@@ -17170,7 +17170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>12.6</v>
       </c>
@@ -17182,107 +17182,107 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>12.6</v>
       </c>
     </row>
-    <row r="128" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>12.6</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129">
         <v>12.6</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130">
         <v>12.6</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131">
         <v>12.6</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132">
         <v>12.6</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133">
         <v>12.6</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134">
         <v>12.6</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135">
         <v>12.6</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136">
         <v>12.6</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137">
         <v>12.6</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138">
         <v>12.6</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139">
         <v>12.6</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140">
         <v>12.6</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141">
         <v>12.6</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142">
         <v>12.6</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B143">
         <v>12.6</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B144">
         <v>12.6</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145">
         <v>12.6</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146">
         <v>12.6</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147">
         <v>12.6</v>
       </c>

</xml_diff>